<commit_message>
Edits in email language
</commit_message>
<xml_diff>
--- a/Supplemental/Spend and Transactions Pivot Tables.xlsx
+++ b/Supplemental/Spend and Transactions Pivot Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ccf779dc7355a40/Documents/Python_Projects/Fetch Rewards Assignment - Data Analyst/Fetch-Rewards-Coding-Assignment/Supplemental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{92D6FA5A-A11B-4A62-9B20-20D9E8BD7FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86EC1BD-2F7B-45B2-98A2-291D52C1CC98}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{92D6FA5A-A11B-4A62-9B20-20D9E8BD7FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FDAEE5A-4891-4D31-9A77-42D078E86E6C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E62EB5EF-B05B-4D17-9C50-041E0ECA9077}"/>
   </bookViews>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="58" r:id="rId4"/>
-    <pivotCache cacheId="62" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -586,9 +586,6 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
     <t>spend</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>Sum of transactions</t>
+  </si>
+  <si>
+    <t>Brands</t>
   </si>
 </sst>
 </file>
@@ -3133,7 +3133,260 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{28579D78-35C8-41D7-A804-2B95C5CD60F7}" name="PivotTable11" cacheId="62" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CAD7A33-637D-4291-947A-9D8FAF409F14}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Brands">
+  <location ref="D2:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField name="Transactions Group" axis="axisRow" showAll="0" sortType="descending">
+      <items count="168">
+        <item x="67"/>
+        <item x="110"/>
+        <item x="118"/>
+        <item x="153"/>
+        <item x="66"/>
+        <item x="142"/>
+        <item x="68"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="109"/>
+        <item x="152"/>
+        <item x="164"/>
+        <item x="19"/>
+        <item x="143"/>
+        <item x="95"/>
+        <item x="18"/>
+        <item x="136"/>
+        <item x="90"/>
+        <item x="46"/>
+        <item x="137"/>
+        <item x="64"/>
+        <item x="10"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="98"/>
+        <item x="13"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="14"/>
+        <item x="104"/>
+        <item x="65"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="141"/>
+        <item x="139"/>
+        <item x="151"/>
+        <item x="70"/>
+        <item x="6"/>
+        <item x="113"/>
+        <item x="85"/>
+        <item x="71"/>
+        <item x="86"/>
+        <item x="23"/>
+        <item x="163"/>
+        <item x="147"/>
+        <item x="3"/>
+        <item x="69"/>
+        <item x="140"/>
+        <item x="24"/>
+        <item x="150"/>
+        <item x="25"/>
+        <item x="89"/>
+        <item x="148"/>
+        <item x="138"/>
+        <item x="88"/>
+        <item x="105"/>
+        <item x="73"/>
+        <item x="22"/>
+        <item x="72"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="21"/>
+        <item x="9"/>
+        <item x="87"/>
+        <item x="149"/>
+        <item x="74"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="130"/>
+        <item x="59"/>
+        <item x="33"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="93"/>
+        <item x="157"/>
+        <item x="94"/>
+        <item x="4"/>
+        <item x="129"/>
+        <item x="135"/>
+        <item x="112"/>
+        <item x="144"/>
+        <item x="32"/>
+        <item x="160"/>
+        <item x="134"/>
+        <item x="80"/>
+        <item x="165"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="26"/>
+        <item x="111"/>
+        <item x="119"/>
+        <item x="91"/>
+        <item x="133"/>
+        <item x="81"/>
+        <item x="27"/>
+        <item x="47"/>
+        <item x="92"/>
+        <item x="28"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="159"/>
+        <item x="31"/>
+        <item x="158"/>
+        <item x="97"/>
+        <item x="154"/>
+        <item x="40"/>
+        <item x="55"/>
+        <item x="155"/>
+        <item x="82"/>
+        <item x="54"/>
+        <item x="0"/>
+        <item x="41"/>
+        <item x="145"/>
+        <item x="166"/>
+        <item x="38"/>
+        <item x="56"/>
+        <item x="156"/>
+        <item x="48"/>
+        <item x="2"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="125"/>
+        <item x="39"/>
+        <item x="124"/>
+        <item x="126"/>
+        <item x="50"/>
+        <item x="122"/>
+        <item x="51"/>
+        <item x="83"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="123"/>
+        <item x="127"/>
+        <item x="120"/>
+        <item x="42"/>
+        <item x="121"/>
+        <item x="96"/>
+        <item x="128"/>
+        <item x="101"/>
+        <item x="49"/>
+        <item x="106"/>
+        <item x="84"/>
+        <item x="161"/>
+        <item x="107"/>
+        <item x="131"/>
+        <item x="103"/>
+        <item x="162"/>
+        <item x="79"/>
+        <item x="99"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="100"/>
+        <item x="43"/>
+        <item x="76"/>
+        <item x="102"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="75"/>
+        <item x="132"/>
+        <item x="108"/>
+        <item x="146"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="7">
+        <item n="All Other Brands" sd="0" x="5"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="1"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of transactions" fld="2" baseField="3" baseItem="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{28579D78-35C8-41D7-A804-2B95C5CD60F7}" name="PivotTable11" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Brands">
   <location ref="A2:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -3373,259 +3626,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of spend" fld="1" baseField="3" baseItem="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E481F3AD-C80A-499C-9466-715E761E9898}" name="PivotTable7" cacheId="58" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A12:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField name="Transactions Group" axis="axisRow" showAll="0" sortType="descending">
-      <items count="168">
-        <item x="67"/>
-        <item x="110"/>
-        <item x="118"/>
-        <item x="153"/>
-        <item x="66"/>
-        <item x="142"/>
-        <item x="68"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="109"/>
-        <item x="152"/>
-        <item x="164"/>
-        <item x="19"/>
-        <item x="143"/>
-        <item x="95"/>
-        <item x="18"/>
-        <item x="136"/>
-        <item x="90"/>
-        <item x="46"/>
-        <item x="137"/>
-        <item x="64"/>
-        <item x="10"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="98"/>
-        <item x="13"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="14"/>
-        <item x="104"/>
-        <item x="65"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="141"/>
-        <item x="139"/>
-        <item x="151"/>
-        <item x="70"/>
-        <item x="6"/>
-        <item x="113"/>
-        <item x="85"/>
-        <item x="71"/>
-        <item x="86"/>
-        <item x="23"/>
-        <item x="163"/>
-        <item x="147"/>
-        <item x="3"/>
-        <item x="69"/>
-        <item x="140"/>
-        <item x="24"/>
-        <item x="150"/>
-        <item x="25"/>
-        <item x="89"/>
-        <item x="148"/>
-        <item x="138"/>
-        <item x="88"/>
-        <item x="105"/>
-        <item x="73"/>
-        <item x="22"/>
-        <item x="72"/>
-        <item x="116"/>
-        <item x="117"/>
-        <item x="21"/>
-        <item x="9"/>
-        <item x="87"/>
-        <item x="149"/>
-        <item x="74"/>
-        <item x="114"/>
-        <item x="115"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="130"/>
-        <item x="59"/>
-        <item x="33"/>
-        <item x="60"/>
-        <item x="61"/>
-        <item x="93"/>
-        <item x="157"/>
-        <item x="94"/>
-        <item x="4"/>
-        <item x="129"/>
-        <item x="135"/>
-        <item x="112"/>
-        <item x="144"/>
-        <item x="32"/>
-        <item x="160"/>
-        <item x="134"/>
-        <item x="80"/>
-        <item x="165"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="26"/>
-        <item x="111"/>
-        <item x="119"/>
-        <item x="91"/>
-        <item x="133"/>
-        <item x="81"/>
-        <item x="27"/>
-        <item x="47"/>
-        <item x="92"/>
-        <item x="28"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="159"/>
-        <item x="31"/>
-        <item x="158"/>
-        <item x="97"/>
-        <item x="154"/>
-        <item x="40"/>
-        <item x="55"/>
-        <item x="155"/>
-        <item x="82"/>
-        <item x="54"/>
-        <item x="0"/>
-        <item x="41"/>
-        <item x="145"/>
-        <item x="166"/>
-        <item x="38"/>
-        <item x="56"/>
-        <item x="156"/>
-        <item x="48"/>
-        <item x="2"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="125"/>
-        <item x="39"/>
-        <item x="124"/>
-        <item x="126"/>
-        <item x="50"/>
-        <item x="122"/>
-        <item x="51"/>
-        <item x="83"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="123"/>
-        <item x="127"/>
-        <item x="120"/>
-        <item x="42"/>
-        <item x="121"/>
-        <item x="96"/>
-        <item x="128"/>
-        <item x="101"/>
-        <item x="49"/>
-        <item x="106"/>
-        <item x="84"/>
-        <item x="161"/>
-        <item x="107"/>
-        <item x="131"/>
-        <item x="103"/>
-        <item x="162"/>
-        <item x="79"/>
-        <item x="99"/>
-        <item x="77"/>
-        <item x="78"/>
-        <item x="100"/>
-        <item x="43"/>
-        <item x="76"/>
-        <item x="102"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="75"/>
-        <item x="132"/>
-        <item x="108"/>
-        <item x="146"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="7">
-        <item n="All Other Brands" sd="0" x="5"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="0"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="1"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of transactions" fld="2" baseField="3" baseItem="4"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3936,151 +3936,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5E745B-90FC-4449-ADA8-4EF1377288C1}">
-  <dimension ref="A2:B19"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="B3" s="3">
         <v>1202629.1000000015</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="3">
+        <v>214325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>20040.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>19390.599999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="3">
         <v>18900</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="3">
         <v>18555.400000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3">
         <v>18362.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3674</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B9" s="3">
         <v>1297878.6000000015</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B13" s="3">
-        <v>214325</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3">
-        <v>4111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
-        <v>3937</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <v>3748</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3">
-        <v>3681</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3">
-        <v>3674</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="3">
+      <c r="E9" s="3">
         <v>233476</v>
       </c>
     </row>
@@ -4104,10 +4082,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
         <v>170</v>
-      </c>
-      <c r="C1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>